<commit_message>
remove unusd conf file, switch to mustache template for all doi records, move some functions
</commit_message>
<xml_diff>
--- a/input/DOI_GEO_Apollo_Reserved_Bundles_20200316.xlsx
+++ b/input/DOI_GEO_Apollo_Reserved_Bundles_20200316.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WINWORD\Data_Prep_HandBook\aaaVer_9_20130225\DOI_20150505\aaDOI_production_submitted_labels\GEO_Apollo_Bundles_reserve_20200316\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loubrieu/PycharmProjects/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD16780F-E119-5B4A-B1B1-F8937A577A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="13665"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27300" windowHeight="13660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -600,26 +601,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="89.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="89.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="49.5" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="41.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -668,7 +669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -691,7 +692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -714,7 +715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -737,7 +738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -760,7 +761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -783,7 +784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -806,7 +807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -829,7 +830,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -852,7 +853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -875,7 +876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
@@ -898,7 +899,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -921,7 +922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -944,7 +945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -967,7 +968,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -990,7 +991,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>25</v>
       </c>
@@ -1084,25 +1085,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I7" r:id="rId3"/>
-    <hyperlink ref="I6" r:id="rId4"/>
-    <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="I4" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>